<commit_message>
photo adult and db-object pev
</commit_message>
<xml_diff>
--- a/forms/app/pev_enfant.xlsx
+++ b/forms/app/pev_enfant.xlsx
@@ -451,6 +451,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">test_context</t>
     </r>
@@ -4752,7 +4753,7 @@
     <numFmt numFmtId="166" formatCode="0"/>
     <numFmt numFmtId="167" formatCode="d\-mmm"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="20">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -4812,24 +4813,11 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -5103,7 +5091,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -5114,7 +5102,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
@@ -5179,11 +5167,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5203,7 +5191,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5267,7 +5255,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5299,7 +5287,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5315,11 +5303,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5363,7 +5351,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="23" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5383,7 +5371,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5399,11 +5387,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5415,7 +5403,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5427,7 +5415,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5463,7 +5451,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5479,19 +5467,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5507,7 +5495,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5519,7 +5507,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -7044,11 +7032,11 @@
   <dimension ref="A1:AA1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
-      <selection pane="bottomRight" activeCell="O78" activeCellId="0" sqref="O78"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.0078125" defaultRowHeight="16.5" zeroHeight="false" outlineLevelRow="1" outlineLevelCol="0"/>
@@ -7266,10 +7254,10 @@
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="0"/>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="G7" s="0"/>
       <c r="J7" s="6"/>
       <c r="K7" s="0"/>
       <c r="L7" s="0"/>
@@ -7288,10 +7276,10 @@
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="0"/>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="0"/>
       <c r="J8" s="6"/>
       <c r="K8" s="0"/>
       <c r="L8" s="0"/>
@@ -7310,10 +7298,10 @@
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="5"/>
+      <c r="G9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G9" s="0"/>
       <c r="J9" s="6"/>
       <c r="K9" s="0"/>
       <c r="L9" s="0"/>
@@ -7330,10 +7318,10 @@
       <c r="C10" s="7"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="5"/>
+      <c r="G10" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="0"/>
       <c r="J10" s="6"/>
       <c r="K10" s="0"/>
       <c r="L10" s="0"/>
@@ -41381,10 +41369,10 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.79296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="13.25"/>
@@ -41426,7 +41414,7 @@
       </c>
       <c r="C2" s="52" t="str">
         <f aca="true">TEXT(YEAR(NOW())-2000, "00") &amp; TEXT(MONTH(NOW()), "00") &amp; TEXT(DAY(NOW()), "00") &amp; TEXT(HOUR(NOW()), "00") &amp; TEXT(MINUTE(NOW()), "00")</f>
-        <v>2302141319</v>
+        <v>2302170944</v>
       </c>
       <c r="D2" s="69"/>
       <c r="E2" s="70"/>
@@ -41459,7 +41447,7 @@
       <selection pane="topLeft" activeCell="A61" activeCellId="0" sqref="A61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="36"/>
@@ -45622,7 +45610,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="36"/>
   </cols>
@@ -45717,7 +45705,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.1171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="1" style="0" width="36"/>
   </cols>

</xml_diff>